<commit_message>
fix: compare response bug fixed
</commit_message>
<xml_diff>
--- a/res/testSceneraios.xlsx
+++ b/res/testSceneraios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\trying\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareProjects\micro-learning\apiTestAutomation\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D24E6E-394D-4534-A2A1-CA9751CA8630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1329F1-20A6-4E88-B21F-FC1682D9BA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{04D79A9D-4EF4-4E8B-BB18-2C541007807D}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{04D79A9D-4EF4-4E8B-BB18-2C541007807D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3AA515B-9148-45F6-909D-F7C1D55E06A2}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: check by field feature added
</commit_message>
<xml_diff>
--- a/res/testSceneraios.xlsx
+++ b/res/testSceneraios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareProjects\micro-learning\apiTestAutomation\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1329F1-20A6-4E88-B21F-FC1682D9BA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE2AD90-A1FC-4C73-AFB9-773BA12A5602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{04D79A9D-4EF4-4E8B-BB18-2C541007807D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{04D79A9D-4EF4-4E8B-BB18-2C541007807D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>scenarioName</t>
   </si>
@@ -118,6 +118,27 @@
     "timestamp": "2023-09-26T13:41:36.057+00:00",
     "error": "something went wrong!"
 }</t>
+  </si>
+  <si>
+    <t>checkOnlyField</t>
+  </si>
+  <si>
+    <t>http://172.19.144.1:8090/mock-handler/api/fields</t>
+  </si>
+  <si>
+    <t>customer.id</t>
+  </si>
+  <si>
+    <t>get and check customer id</t>
+  </si>
+  <si>
+    <t>get and check masterno</t>
+  </si>
+  <si>
+    <t>….</t>
+  </si>
+  <si>
+    <t>masterno</t>
   </si>
 </sst>
 </file>
@@ -498,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3AA515B-9148-45F6-909D-F7C1D55E06A2}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,9 +532,10 @@
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -532,8 +554,11 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -550,7 +575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -570,7 +595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -587,7 +612,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -602,6 +627,46 @@
       </c>
       <c r="F5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2">
+        <v>123</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -611,8 +676,10 @@
     <hyperlink ref="E3" r:id="rId2" xr:uid="{777D9ADF-2D39-4500-972B-14E916028AEF}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{6A3B3571-F91C-452F-9D8B-3DB207830593}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{9C23550E-7489-4704-AD23-D307811CE2EC}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{7A1EC64A-D61C-44ED-AE16-415ECA2D09AF}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{254EE700-F25A-4D51-872B-E7D7B8F28F8F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>